<commit_message>
added issues to to-do list
</commit_message>
<xml_diff>
--- a/To-do List - Progress Tracker.xlsx
+++ b/To-do List - Progress Tracker.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="150" windowWidth="13395" windowHeight="4935"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Task</t>
   </si>
@@ -106,13 +106,22 @@
   </si>
   <si>
     <t>Server</t>
+  </si>
+  <si>
+    <t>Setup Azure account</t>
+  </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>Install Azure SDK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,6 +332,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -401,6 +415,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -435,6 +450,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -610,27 +626,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E1" s="1">
         <f ca="1">NOW()</f>
-        <v>41069.639564930556</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="33.75">
+        <v>41073.468588310185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -639,7 +655,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="18.75">
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -648,14 +664,14 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="26.25" thickBot="1">
+    <row r="5" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>1</v>
       </c>
@@ -672,7 +688,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -683,7 +699,7 @@
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="28">
         <v>1</v>
       </c>
@@ -698,7 +714,7 @@
       </c>
       <c r="E7" s="14"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <v>2</v>
       </c>
@@ -707,7 +723,7 @@
       <c r="D8" s="26"/>
       <c r="E8" s="15"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="28">
         <v>3</v>
       </c>
@@ -716,7 +732,7 @@
       <c r="D9" s="25"/>
       <c r="E9" s="16"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
         <v>4</v>
       </c>
@@ -725,7 +741,7 @@
       <c r="D10" s="26"/>
       <c r="E10" s="17"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="28">
         <v>5</v>
       </c>
@@ -734,7 +750,7 @@
       <c r="D11" s="25"/>
       <c r="E11" s="16"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>6</v>
       </c>
@@ -743,7 +759,7 @@
       <c r="D12" s="26"/>
       <c r="E12" s="17"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="28">
         <v>7</v>
       </c>
@@ -752,7 +768,7 @@
       <c r="D13" s="25"/>
       <c r="E13" s="16"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="29">
         <v>8</v>
       </c>
@@ -761,7 +777,7 @@
       <c r="D14" s="26"/>
       <c r="E14" s="17"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="28">
         <v>9</v>
       </c>
@@ -770,7 +786,7 @@
       <c r="D15" s="25"/>
       <c r="E15" s="16"/>
     </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1">
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29">
         <v>10</v>
       </c>
@@ -779,7 +795,7 @@
       <c r="D16" s="26"/>
       <c r="E16" s="17"/>
     </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1">
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="30" t="s">
         <v>12</v>
       </c>
@@ -790,7 +806,7 @@
       <c r="D17" s="27"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="28">
         <v>1</v>
       </c>
@@ -807,7 +823,7 @@
         <v>41069</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <v>2</v>
       </c>
@@ -820,7 +836,7 @@
       <c r="D19" s="26"/>
       <c r="E19" s="19"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="28">
         <v>3</v>
       </c>
@@ -829,7 +845,7 @@
       <c r="D20" s="25"/>
       <c r="E20" s="18"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
         <v>4</v>
       </c>
@@ -838,7 +854,7 @@
       <c r="D21" s="26"/>
       <c r="E21" s="19"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="28">
         <v>5</v>
       </c>
@@ -847,7 +863,7 @@
       <c r="D22" s="25"/>
       <c r="E22" s="18"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
         <v>6</v>
       </c>
@@ -856,7 +872,7 @@
       <c r="D23" s="26"/>
       <c r="E23" s="19"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="28">
         <v>7</v>
       </c>
@@ -865,7 +881,7 @@
       <c r="D24" s="25"/>
       <c r="E24" s="18"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="29">
         <v>8</v>
       </c>
@@ -874,7 +890,7 @@
       <c r="D25" s="26"/>
       <c r="E25" s="19"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="28">
         <v>9</v>
       </c>
@@ -883,7 +899,7 @@
       <c r="D26" s="25"/>
       <c r="E26" s="18"/>
     </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1">
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="29">
         <v>10</v>
       </c>
@@ -892,7 +908,7 @@
       <c r="D27" s="26"/>
       <c r="E27" s="19"/>
     </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1">
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="30" t="s">
         <v>15</v>
       </c>
@@ -903,7 +919,7 @@
       <c r="D28" s="27"/>
       <c r="E28" s="20"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="28">
         <v>1</v>
       </c>
@@ -912,7 +928,7 @@
       <c r="D29" s="25"/>
       <c r="E29" s="18"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
         <v>2</v>
       </c>
@@ -921,7 +937,7 @@
       <c r="D30" s="26"/>
       <c r="E30" s="19"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="28">
         <v>3</v>
       </c>
@@ -930,7 +946,7 @@
       <c r="D31" s="25"/>
       <c r="E31" s="21"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
         <v>4</v>
       </c>
@@ -939,7 +955,7 @@
       <c r="D32" s="26"/>
       <c r="E32" s="22"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="28">
         <v>5</v>
       </c>
@@ -948,7 +964,7 @@
       <c r="D33" s="25"/>
       <c r="E33" s="21"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="29">
         <v>6</v>
       </c>
@@ -957,7 +973,7 @@
       <c r="D34" s="26"/>
       <c r="E34" s="22"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="28">
         <v>7</v>
       </c>
@@ -966,7 +982,7 @@
       <c r="D35" s="25"/>
       <c r="E35" s="21"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="29">
         <v>8</v>
       </c>
@@ -975,7 +991,7 @@
       <c r="D36" s="26"/>
       <c r="E36" s="22"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="28">
         <v>9</v>
       </c>
@@ -984,7 +1000,7 @@
       <c r="D37" s="25"/>
       <c r="E37" s="21"/>
     </row>
-    <row r="38" spans="1:5" ht="15.75" thickBot="1">
+    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="29">
         <v>10</v>
       </c>
@@ -993,7 +1009,7 @@
       <c r="D38" s="26"/>
       <c r="E38" s="22"/>
     </row>
-    <row r="39" spans="1:5" ht="15.75" thickBot="1">
+    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="30" t="s">
         <v>10</v>
       </c>
@@ -1004,7 +1020,7 @@
       <c r="D39" s="27"/>
       <c r="E39" s="20"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="28">
         <v>1</v>
       </c>
@@ -1021,7 +1037,7 @@
         <v>41069</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="29">
         <v>2</v>
       </c>
@@ -1038,7 +1054,7 @@
         <v>41069</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="28">
         <v>3</v>
       </c>
@@ -1055,7 +1071,7 @@
         <v>41069</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="29">
         <v>4</v>
       </c>
@@ -1064,7 +1080,7 @@
       <c r="D43" s="26"/>
       <c r="E43" s="22"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="28">
         <v>5</v>
       </c>
@@ -1073,7 +1089,7 @@
       <c r="D44" s="25"/>
       <c r="E44" s="21"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="29">
         <v>6</v>
       </c>
@@ -1082,7 +1098,7 @@
       <c r="D45" s="26"/>
       <c r="E45" s="22"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="28">
         <v>7</v>
       </c>
@@ -1091,7 +1107,7 @@
       <c r="D46" s="25"/>
       <c r="E46" s="21"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="29">
         <v>8</v>
       </c>
@@ -1100,7 +1116,7 @@
       <c r="D47" s="26"/>
       <c r="E47" s="22"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="28">
         <v>9</v>
       </c>
@@ -1109,7 +1125,7 @@
       <c r="D48" s="25"/>
       <c r="E48" s="21"/>
     </row>
-    <row r="49" spans="1:5" ht="15.75" thickBot="1">
+    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="29">
         <v>10</v>
       </c>
@@ -1118,7 +1134,7 @@
       <c r="D49" s="26"/>
       <c r="E49" s="22"/>
     </row>
-    <row r="50" spans="1:5" ht="15.75" thickBot="1">
+    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="30" t="s">
         <v>16</v>
       </c>
@@ -1129,7 +1145,7 @@
       <c r="D50" s="27"/>
       <c r="E50" s="20"/>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="28">
         <v>1</v>
       </c>
@@ -1140,7 +1156,7 @@
       <c r="D51" s="25"/>
       <c r="E51" s="18"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="29">
         <v>2</v>
       </c>
@@ -1151,7 +1167,7 @@
       <c r="D52" s="26"/>
       <c r="E52" s="19"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="28">
         <v>3</v>
       </c>
@@ -1162,7 +1178,7 @@
       <c r="D53" s="25"/>
       <c r="E53" s="21"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="29">
         <v>4</v>
       </c>
@@ -1171,7 +1187,7 @@
       <c r="D54" s="26"/>
       <c r="E54" s="22"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="28">
         <v>5</v>
       </c>
@@ -1180,7 +1196,7 @@
       <c r="D55" s="25"/>
       <c r="E55" s="21"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="29">
         <v>6</v>
       </c>
@@ -1189,7 +1205,7 @@
       <c r="D56" s="26"/>
       <c r="E56" s="22"/>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="28">
         <v>7</v>
       </c>
@@ -1198,7 +1214,7 @@
       <c r="D57" s="25"/>
       <c r="E57" s="21"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="29">
         <v>8</v>
       </c>
@@ -1207,7 +1223,7 @@
       <c r="D58" s="26"/>
       <c r="E58" s="22"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="28">
         <v>9</v>
       </c>
@@ -1216,7 +1232,7 @@
       <c r="D59" s="25"/>
       <c r="E59" s="21"/>
     </row>
-    <row r="60" spans="1:5" ht="15.75" thickBot="1">
+    <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="29">
         <v>10</v>
       </c>
@@ -1225,7 +1241,7 @@
       <c r="D60" s="26"/>
       <c r="E60" s="22"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" thickBot="1">
+    <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="30" t="s">
         <v>16</v>
       </c>
@@ -1236,25 +1252,37 @@
       <c r="D61" s="27"/>
       <c r="E61" s="20"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="28">
         <v>1</v>
       </c>
-      <c r="B62" s="9"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="18"/>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="B62" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D62" s="25">
+        <v>1</v>
+      </c>
+      <c r="E62" s="18">
+        <v>41073</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="29">
         <v>2</v>
       </c>
-      <c r="B63" s="11"/>
-      <c r="C63" s="12"/>
+      <c r="B63" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>7</v>
+      </c>
       <c r="D63" s="26"/>
       <c r="E63" s="19"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="28">
         <v>3</v>
       </c>
@@ -1263,7 +1291,7 @@
       <c r="D64" s="25"/>
       <c r="E64" s="21"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="29">
         <v>4</v>
       </c>
@@ -1272,7 +1300,7 @@
       <c r="D65" s="26"/>
       <c r="E65" s="22"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="28">
         <v>5</v>
       </c>
@@ -1281,7 +1309,7 @@
       <c r="D66" s="25"/>
       <c r="E66" s="21"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="29">
         <v>6</v>
       </c>
@@ -1290,7 +1318,7 @@
       <c r="D67" s="26"/>
       <c r="E67" s="22"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="28">
         <v>7</v>
       </c>
@@ -1299,7 +1327,7 @@
       <c r="D68" s="25"/>
       <c r="E68" s="21"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="29">
         <v>8</v>
       </c>
@@ -1308,7 +1336,7 @@
       <c r="D69" s="26"/>
       <c r="E69" s="22"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="28">
         <v>9</v>
       </c>
@@ -1317,7 +1345,7 @@
       <c r="D70" s="25"/>
       <c r="E70" s="21"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="29">
         <v>10</v>
       </c>
@@ -1333,24 +1361,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated To do list with action points
</commit_message>
<xml_diff>
--- a/To-do List - Progress Tracker.xlsx
+++ b/To-do List - Progress Tracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>Task</t>
   </si>
@@ -127,13 +127,43 @@
   </si>
   <si>
     <t>Add new Azure website</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Use LINQ builder to create schema</t>
+  </si>
+  <si>
+    <t>Design Use cases</t>
+  </si>
+  <si>
+    <t>Tidy up ward numbers vs. names</t>
+  </si>
+  <si>
+    <t>31/06/2012</t>
+  </si>
+  <si>
+    <t>Update main document with use cases</t>
+  </si>
+  <si>
+    <t>Identify Excel parser</t>
+  </si>
+  <si>
+    <t>Write parsers for elec. and contrib.</t>
+  </si>
+  <si>
+    <t>Investigate data storage on Azure</t>
+  </si>
+  <si>
+    <t>Write formal intro and content</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +197,14 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -248,9 +286,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
@@ -293,12 +330,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -308,12 +339,6 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -337,6 +362,30 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -642,761 +691,809 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E1" s="1">
+      <c r="E1" s="31">
         <f ca="1">NOW()</f>
-        <v>41074.514472106479</v>
+        <v>41092.509014467592</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="19" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="28">
+      <c r="A7" s="23">
         <v>1</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="20">
         <v>0.85</v>
       </c>
-      <c r="E7" s="14"/>
+      <c r="E7" s="13"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="29">
+      <c r="A8" s="24">
         <v>2</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="15"/>
+      <c r="B8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
+      <c r="A9" s="23">
         <v>3</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="16"/>
+      <c r="B9" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="15" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="29">
+      <c r="A10" s="24">
         <v>4</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="17"/>
+      <c r="B10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="16">
+        <v>41094</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="28">
+      <c r="A11" s="23">
         <v>5</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="16"/>
+      <c r="B11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="29">
+      <c r="A12" s="24">
         <v>6</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="17"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="14"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="28">
+      <c r="A13" s="23">
         <v>7</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="16"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="29">
+      <c r="A14" s="24">
         <v>8</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="17"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="14"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="28">
+      <c r="A15" s="23">
         <v>9</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="16"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="13"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="29">
+      <c r="A16" s="24">
         <v>10</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="17"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="14"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="8"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="28">
+      <c r="A18" s="23">
         <v>1</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="20">
         <v>1</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="15">
         <v>41069</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="29">
+      <c r="A19" s="26">
         <v>2</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="19"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="30" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="28">
+      <c r="A20" s="23">
         <v>3</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="20">
         <v>1</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="15">
         <v>41074</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="29">
+      <c r="A21" s="24">
         <v>4</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="19"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="16"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="28">
+      <c r="A22" s="23">
         <v>5</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="18"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="15"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="29">
+      <c r="A23" s="24">
         <v>6</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="19"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="16"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="28">
+      <c r="A24" s="23">
         <v>7</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="18"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="15"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="29">
+      <c r="A25" s="24">
         <v>8</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="19"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="16"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="28">
+      <c r="A26" s="23">
         <v>9</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="18"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="15"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="29">
+      <c r="A27" s="24">
         <v>10</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="19"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="16"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="20"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="17"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="28">
+      <c r="A29" s="23">
         <v>1</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="20">
         <v>1</v>
       </c>
-      <c r="E29" s="18">
+      <c r="E29" s="15">
         <v>41073</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="29">
+      <c r="A30" s="24">
         <v>2</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="26"/>
-      <c r="E30" s="19">
+      <c r="D30" s="21">
+        <v>1</v>
+      </c>
+      <c r="E30" s="16">
         <v>41074</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="28">
+      <c r="A31" s="23">
         <v>3</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="21"/>
+      <c r="B31" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="20">
+        <v>1</v>
+      </c>
+      <c r="E31" s="15">
+        <v>41074</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="29">
+      <c r="A32" s="24">
         <v>4</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="22"/>
+      <c r="B32" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="21"/>
+      <c r="E32" s="16">
+        <v>41094</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="28">
+      <c r="A33" s="23">
         <v>5</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="21"/>
+      <c r="B33" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="20"/>
+      <c r="E33" s="16">
+        <v>41094</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="29">
+      <c r="A34" s="24">
         <v>6</v>
       </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="22"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="16"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="28">
+      <c r="A35" s="23">
         <v>7</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="21"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="15"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="29">
+      <c r="A36" s="24">
         <v>8</v>
       </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="22"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="16"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="28">
+      <c r="A37" s="23">
         <v>9</v>
       </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="21"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="15"/>
     </row>
     <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="29">
+      <c r="A38" s="24">
         <v>10</v>
       </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="22"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="16"/>
     </row>
     <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="20"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="17"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="28">
+      <c r="A40" s="23">
         <v>1</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D40" s="25">
+      <c r="D40" s="20">
         <v>1</v>
       </c>
-      <c r="E40" s="18">
+      <c r="E40" s="15">
         <v>41069</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="29">
+      <c r="A41" s="24">
         <v>2</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="26">
+      <c r="D41" s="21">
         <v>0</v>
       </c>
-      <c r="E41" s="19">
+      <c r="E41" s="16">
         <v>41069</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="28">
+      <c r="A42" s="23">
         <v>3</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="25">
+      <c r="D42" s="20">
         <v>0</v>
       </c>
-      <c r="E42" s="18">
+      <c r="E42" s="15">
         <v>41069</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="29">
+      <c r="A43" s="24">
         <v>4</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="22"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="16"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="28">
+      <c r="A44" s="23">
         <v>5</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="21"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="15"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="29">
+      <c r="A45" s="24">
         <v>6</v>
       </c>
-      <c r="B45" s="11"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="22"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="16"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="28">
+      <c r="A46" s="23">
         <v>7</v>
       </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="21"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="15"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="29">
+      <c r="A47" s="24">
         <v>8</v>
       </c>
-      <c r="B47" s="11"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="22"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="16"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="28">
+      <c r="A48" s="23">
         <v>9</v>
       </c>
-      <c r="B48" s="9"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="21"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="15"/>
     </row>
     <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="29">
+      <c r="A49" s="24">
         <v>10</v>
       </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="22"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="16"/>
     </row>
     <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="30" t="s">
+      <c r="A50" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C50" s="13"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="20"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="17"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="28">
+      <c r="A51" s="23">
         <v>1</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C51" s="10"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="18"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="15"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="29">
+      <c r="A52" s="24">
         <v>2</v>
       </c>
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C52" s="12"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="19"/>
+      <c r="C52" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" s="21"/>
+      <c r="E52" s="16"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="28">
+      <c r="A53" s="23">
         <v>3</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C53" s="10"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="21"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="15"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="29">
+      <c r="A54" s="24">
         <v>4</v>
       </c>
-      <c r="B54" s="11"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="22"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="16"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="28">
+      <c r="A55" s="23">
         <v>5</v>
       </c>
-      <c r="B55" s="9"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="21"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="15"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="29">
+      <c r="A56" s="24">
         <v>6</v>
       </c>
-      <c r="B56" s="11"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="22"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="16"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="28">
+      <c r="A57" s="23">
         <v>7</v>
       </c>
-      <c r="B57" s="9"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="21"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="15"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="29">
+      <c r="A58" s="24">
         <v>8</v>
       </c>
-      <c r="B58" s="11"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="22"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="16"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="28">
+      <c r="A59" s="23">
         <v>9</v>
       </c>
-      <c r="B59" s="9"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="21"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="15"/>
     </row>
     <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="29">
+      <c r="A60" s="24">
         <v>10</v>
       </c>
-      <c r="B60" s="11"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="26"/>
-      <c r="E60" s="22"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="16"/>
     </row>
     <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="30" t="s">
+      <c r="A61" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B61" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C61" s="13"/>
-      <c r="D61" s="27"/>
-      <c r="E61" s="20"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="17"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="28">
+      <c r="A62" s="23">
         <v>1</v>
       </c>
-      <c r="B62" s="9" t="s">
+      <c r="B62" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C62" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D62" s="25">
+      <c r="D62" s="20">
         <v>1</v>
       </c>
-      <c r="E62" s="18">
+      <c r="E62" s="15">
         <v>41073</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="29">
+      <c r="A63" s="24">
         <v>2</v>
       </c>
-      <c r="B63" s="11" t="s">
+      <c r="B63" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C63" s="12" t="s">
+      <c r="C63" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D63" s="26">
-        <v>0.5</v>
-      </c>
-      <c r="E63" s="19"/>
+      <c r="D63" s="21">
+        <v>1</v>
+      </c>
+      <c r="E63" s="16"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="28">
+      <c r="A64" s="23">
         <v>3</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C64" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D64" s="25">
+      <c r="D64" s="20">
         <v>1</v>
       </c>
-      <c r="E64" s="18">
+      <c r="E64" s="15">
         <v>41074</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="29">
+      <c r="A65" s="24">
         <v>4</v>
       </c>
-      <c r="B65" s="11"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="26"/>
-      <c r="E65" s="22"/>
+      <c r="B65" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C65" s="11"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="16">
+        <v>41091</v>
+      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="28">
+      <c r="A66" s="23">
         <v>5</v>
       </c>
-      <c r="B66" s="9"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="21"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="15"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="29">
+      <c r="A67" s="24">
         <v>6</v>
       </c>
-      <c r="B67" s="11"/>
-      <c r="C67" s="12"/>
-      <c r="D67" s="26"/>
-      <c r="E67" s="22"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="16"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="28">
+      <c r="A68" s="23">
         <v>7</v>
       </c>
-      <c r="B68" s="9"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="21"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="15"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="29">
+      <c r="A69" s="24">
         <v>8</v>
       </c>
-      <c r="B69" s="11"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="26"/>
-      <c r="E69" s="22"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="16"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="28">
+      <c r="A70" s="23">
         <v>9</v>
       </c>
-      <c r="B70" s="9"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="21"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="15"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="29">
+      <c r="A71" s="24">
         <v>10</v>
       </c>
-      <c r="B71" s="11"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="26"/>
-      <c r="E71" s="22"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated to-do, new lookup & usecases
Sample report/usecases/layouts & Postal code V Ward No. Lookup file
</commit_message>
<xml_diff>
--- a/To-do List - Progress Tracker.xlsx
+++ b/To-do List - Progress Tracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>Task</t>
   </si>
@@ -135,15 +135,6 @@
     <t>Use LINQ builder to create schema</t>
   </si>
   <si>
-    <t>Design Use cases</t>
-  </si>
-  <si>
-    <t>Tidy up ward numbers vs. names</t>
-  </si>
-  <si>
-    <t>31/06/2012</t>
-  </si>
-  <si>
     <t>Update main document with use cases</t>
   </si>
   <si>
@@ -160,6 +151,12 @@
   </si>
   <si>
     <t>DB</t>
+  </si>
+  <si>
+    <t>Design Use cases/sample reports layout</t>
+  </si>
+  <si>
+    <t>Build lookup file-postcode V ward #</t>
   </si>
 </sst>
 </file>
@@ -691,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -705,7 +702,7 @@
     <row r="1" spans="1:5">
       <c r="E1" s="31">
         <f ca="1">NOW()</f>
-        <v>41092.77636747685</v>
+        <v>41092.908545601851</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="33.75">
@@ -774,19 +771,21 @@
       </c>
       <c r="E7" s="13"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="24">
         <v>2</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="14" t="s">
-        <v>41</v>
+      <c r="D8" s="21">
+        <v>1</v>
+      </c>
+      <c r="E8" s="16">
+        <v>41092</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -794,14 +793,16 @@
         <v>3</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="15" t="s">
-        <v>41</v>
+      <c r="D9" s="20">
+        <v>1</v>
+      </c>
+      <c r="E9" s="15">
+        <v>41092</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -809,14 +810,16 @@
         <v>4</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="21"/>
+      <c r="D10" s="21">
+        <v>1</v>
+      </c>
       <c r="E10" s="16">
-        <v>41094</v>
+        <v>41092</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -824,10 +827,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="15">
@@ -1069,7 +1072,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>30</v>
@@ -1084,7 +1087,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>30</v>
@@ -1438,7 +1441,7 @@
         <v>4</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C65" s="11"/>
       <c r="D65" s="21"/>

</xml_diff>